<commit_message>
update diversity with charts
</commit_message>
<xml_diff>
--- a/resources/diversity.xlsx
+++ b/resources/diversity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaoyan/DATA/work/rc_msbi/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiao\git\rc_msbi\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135A4352-3D07-48EA-8EC3-5FD26268EE75}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ES Ethnicity" sheetId="1" r:id="rId1"/>
@@ -17,8 +18,22 @@
     <sheet name="MS Ethnicity" sheetId="2" r:id="rId3"/>
     <sheet name="MS Economy" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'ES Economy'!$A$2:$A$5</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'ES Economy'!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'ES Economy'!$B$2:$B$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'ES Economy'!$A$2:$A$5</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'ES Economy'!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'ES Economy'!$B$2:$B$5</definedName>
+  </definedNames>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Elementary school</t>
   </si>
@@ -179,9 +194,6 @@
     <t>Data from https://www.schooldigger.com/</t>
   </si>
   <si>
-    <t>Our proposal (stoller)</t>
-  </si>
-  <si>
     <t>our proposal (timberline)</t>
   </si>
   <si>
@@ -189,12 +201,15 @@
   </si>
   <si>
     <t>Our proposal(stroller)</t>
+  </si>
+  <si>
+    <t>Proposed Stoller Ethnic Diversity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -395,6 +410,1951 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ES Ethnicity'!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Proposed Stoller Ethnic Diversity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ES Ethnicity'!$B$28:$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>White</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hispanic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Two or more races</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>African American</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>American Indian</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pacific Islander</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ES Ethnicity'!$B$30:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38899999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43885714285714278</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4428571428571431E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8571428571428566E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1571428571428571E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4285714285714288E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8571428571428572E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA74-450C-B6B9-00DA8EDFC934}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ES Economy'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Free/discounted lunch recipients</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ES Economy'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Rock Creek</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Springville</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sato</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Jacob Wismer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ES Economy'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.215</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.129</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00%">
+                  <c:v>5.6000000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-92E4-457F-BEDE-386CFB5CB179}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1505868543"/>
+        <c:axId val="1580509327"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1505868543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1580509327"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1580509327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1505868543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2491740</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C588514-B51B-4267-97BC-BC53F5FB767A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>224790</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927D7A9E-7502-431D-B61E-3576B6A160BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -657,23 +2617,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="5" max="5" width="16.296875" customWidth="1"/>
     <col min="6" max="7" width="16" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +2662,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -728,7 +2688,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -754,7 +2714,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -778,7 +2738,7 @@
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -802,7 +2762,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -828,7 +2788,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -854,7 +2814,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -877,93 +2837,116 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -996,9 +2979,9 @@
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B30" s="10">
         <f>(SUM(B2:B4) + B5/2)/3.5</f>
@@ -1029,9 +3012,9 @@
         <v>3.8571428571428572E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="10">
         <f>(SUM(B6:B8) + B5/2)/3.5</f>
@@ -1062,7 +3045,7 @@
         <v>3.5714285714285713E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1071,7 +3054,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1104,7 +3087,7 @@
         <v>2.6666666666666666E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1140,25 +3123,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="2" max="2" width="27.296875" customWidth="1"/>
+    <col min="10" max="10" width="15.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +3150,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1174,7 +3158,7 @@
         <v>0.215</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +3166,7 @@
         <v>0.159</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1190,7 +3174,7 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1198,7 +3182,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1206,7 +3190,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +3198,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1222,93 +3206,93 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1317,25 +3301,25 @@
         <v>0.12280000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="10">
         <f>(SUM(B2:B4) + B5/2)/3.5</f>
         <v>0.15171428571428572</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="10">
         <f>(SUM(B6:B8) + B5/2)/3.5</f>
         <v>8.9142857142857163E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1344,7 +3328,7 @@
         <v>0.11466666666666668</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1353,30 +3337,32 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1402,7 +3388,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +3414,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
@@ -1454,49 +3440,49 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
@@ -1507,20 +3493,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1529,7 +3515,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
@@ -1538,7 +3524,7 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
@@ -1547,49 +3533,49 @@
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>36</v>
       </c>

</xml_diff>